<commit_message>
Rename transfer file, update package M-Print® PRO
</commit_message>
<xml_diff>
--- a/prog_data.xlsx
+++ b/prog_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr codeName="ЭтаКнига"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proj\MarkV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211F9F47-E36A-40FB-9A2B-287ABA30F898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C2FC1A-37A4-40E9-A47D-414C20C75024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="17772" windowHeight="16620" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="396" yWindow="720" windowWidth="18564" windowHeight="13932" tabRatio="1000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Пути" sheetId="5" r:id="rId1"/>
@@ -100,9 +100,6 @@
     <t>трубка термоусаживаемая</t>
   </si>
   <si>
-    <t>C:\ProgramData\weidmueller\M-Print PRO\shared\filter\ОБЪЕКТ.bis</t>
-  </si>
-  <si>
     <t>ЗПО</t>
   </si>
   <si>
@@ -355,7 +352,10 @@
     <t>transfer_file_name</t>
   </si>
   <si>
-    <t>ОБЪЕКТ.xls</t>
+    <t>transfer_file.xls</t>
+  </si>
+  <si>
+    <t>C:\ProgramData\weidmueller\M-Print PRO\shared\filter\import_transfer_file.bis</t>
   </si>
 </sst>
 </file>
@@ -749,15 +749,15 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -811,16 +811,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -828,16 +828,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -845,7 +845,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
@@ -879,10 +879,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
@@ -922,103 +922,103 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1042,7 +1042,7 @@
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1070,7 +1070,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -1081,7 +1081,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
@@ -1089,7 +1089,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -1105,18 +1105,18 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
         <v>107</v>
-      </c>
-      <c r="B8" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1152,38 +1152,38 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>56</v>
       </c>
-      <c r="D1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
         <v>60</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1192,21 +1192,21 @@
         <v>1513250000</v>
       </c>
       <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
         <v>63</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
         <v>64</v>
-      </c>
-      <c r="F3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1215,21 +1215,21 @@
         <v>1513270000</v>
       </c>
       <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
         <v>66</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" t="s">
         <v>67</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1238,21 +1238,21 @@
         <v>1513290000</v>
       </c>
       <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
         <v>69</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" t="s">
         <v>70</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1261,21 +1261,21 @@
         <v>1513320000</v>
       </c>
       <c r="D6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
         <v>73</v>
-      </c>
-      <c r="F6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1284,15 +1284,15 @@
         <v>1609801044</v>
       </c>
       <c r="D7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
         <v>75</v>
-      </c>
-      <c r="F7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1301,15 +1301,15 @@
         <v>1059780000</v>
       </c>
       <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
         <v>77</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -1318,15 +1318,15 @@
         <v>2005500000</v>
       </c>
       <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s">
         <v>80</v>
-      </c>
-      <c r="F9" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>3</v>
@@ -1335,15 +1335,15 @@
         <v>2006140000</v>
       </c>
       <c r="D10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" t="s">
         <v>83</v>
-      </c>
-      <c r="F10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -1352,15 +1352,15 @@
         <v>1327830000</v>
       </c>
       <c r="D11" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s">
         <v>86</v>
-      </c>
-      <c r="F11" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
         <v>3</v>
@@ -1369,10 +1369,10 @@
         <v>1327800000</v>
       </c>
       <c r="D12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" t="s">
         <v>89</v>
-      </c>
-      <c r="F12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1386,13 +1386,13 @@
         <v>2539400000</v>
       </c>
       <c r="D13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" t="s">
         <v>91</v>
-      </c>
-      <c r="F13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G13" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1406,13 +1406,13 @@
         <v>2539380000</v>
       </c>
       <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
         <v>93</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>94</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1426,13 +1426,13 @@
         <v>2539390000</v>
       </c>
       <c r="D15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" t="s">
         <v>96</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>97</v>
-      </c>
-      <c r="G15" t="s">
-        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>